<commit_message>
slides: terminal, others rounded out ; example directory tree
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="540" windowWidth="13000" windowHeight="8000" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="560" windowWidth="13000" windowHeight="8000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,10 +369,10 @@
         <v>3</v>
       </c>
       <c r="C1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -386,10 +386,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -409,7 +409,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -435,10 +435,10 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -504,10 +504,10 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>3</v>

</xml_diff>

<commit_message>
slides: try-except-finally added to review ; exercises: terminal and imports
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="560" windowWidth="13000" windowHeight="8000" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="880" windowWidth="13000" windowHeight="8000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,7 +369,7 @@
         <v>3</v>
       </c>
       <c r="C1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1">
         <v>9</v>
@@ -392,7 +392,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -409,10 +409,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -435,7 +435,7 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -501,13 +501,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>3</v>

</xml_diff>

<commit_message>
slides: minor slide revisions ; survey results now reflect 2021 questionnaire
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrobeard/Work/Teaching/OSUAstroSURP2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrobeard/Work/Teaching/PythonBootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0733EF3-0A82-0D4E-B806-A0A26EC5C0F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="880" windowWidth="13000" windowHeight="8000" tabRatio="500"/>
+    <workbookView xWindow="-24200" yWindow="3060" windowWidth="16620" windowHeight="10200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,24 +28,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A </t>
   </si>
   <si>
     <t>A-B</t>
   </si>
   <si>
-    <t>C-E</t>
+    <t>B-C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A-E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -85,6 +92,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -352,30 +362,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -386,13 +396,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -409,25 +419,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>3</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -438,7 +448,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -455,71 +465,48 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slides: updated survey responses
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astrobeard/Work/Teaching/PythonBootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0733EF3-0A82-0D4E-B806-A0A26EC5C0F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8639CC1D-6588-8041-A6CE-1F80CB59C7DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24200" yWindow="3060" windowWidth="16620" windowHeight="10200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23780" yWindow="5200" windowWidth="16620" windowHeight="10200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -382,7 +382,7 @@
         <v>4</v>
       </c>
       <c r="D1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -399,7 +399,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -419,7 +419,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -468,7 +468,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -491,7 +491,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>5</v>

</xml_diff>